<commit_message>
Updated for version 2
</commit_message>
<xml_diff>
--- a/LTRDCN-2147.xlsx
+++ b/LTRDCN-2147.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cisco-my.sharepoint.com/personal/richwats_cisco_com/Documents/SE/Dev/NDFC/ndfc-automation-lab-v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{6AFC0E8B-1328-9D40-99D0-F7730C1ABE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8AB0145-643D-7640-90B7-FB329B42ABA3}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{6AFC0E8B-1328-9D40-99D0-F7730C1ABE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03D32C9F-5E0A-F24E-A394-2081033B688D}"/>
   <bookViews>
-    <workbookView xWindow="53320" yWindow="5080" windowWidth="28040" windowHeight="17440" xr2:uid="{CFD4EBC6-3068-5443-B5EF-FB22B87CAC8A}"/>
+    <workbookView xWindow="1680" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{CFD4EBC6-3068-5443-B5EF-FB22B87CAC8A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="OOB-MGMT" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,74 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
-  <si>
-    <t>198.18.192.1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>VLAN 101 GW</t>
   </si>
   <si>
-    <t>198.18.192.2</t>
-  </si>
-  <si>
-    <t>198.18.192.3</t>
-  </si>
-  <si>
-    <t>198.18.192.4</t>
-  </si>
-  <si>
-    <t>198.18.192.5</t>
-  </si>
-  <si>
-    <t>198.18.192.6</t>
-  </si>
-  <si>
-    <t>198.18.192.7</t>
-  </si>
-  <si>
-    <t>198.18.192.8</t>
-  </si>
-  <si>
-    <t>198.18.192.9</t>
-  </si>
-  <si>
-    <t>198.18.192.10</t>
-  </si>
-  <si>
-    <t>198.18.192.11</t>
-  </si>
-  <si>
-    <t>198.18.192.12</t>
-  </si>
-  <si>
-    <t>198.18.192.13</t>
-  </si>
-  <si>
-    <t>198.18.192.14</t>
-  </si>
-  <si>
-    <t>198.18.192.15</t>
-  </si>
-  <si>
-    <t>198.18.192.16</t>
-  </si>
-  <si>
-    <t>198.18.192.17</t>
-  </si>
-  <si>
-    <t>198.18.192.18</t>
-  </si>
-  <si>
-    <t>198.18.192.19</t>
-  </si>
-  <si>
-    <t>198.18.192.20</t>
-  </si>
-  <si>
-    <t>198.18.192.21</t>
-  </si>
-  <si>
     <t>DC1-SPINE-1</t>
   </si>
   <si>
@@ -122,12 +59,6 @@
     <t>DC1-LEAF-4</t>
   </si>
   <si>
-    <t>DC1-LEAF-5</t>
-  </si>
-  <si>
-    <t>DC1-LEAF-6</t>
-  </si>
-  <si>
     <t>DC1-ABGW-1</t>
   </si>
   <si>
@@ -146,72 +77,9 @@
     <t>VRF2-NET1-HOST1</t>
   </si>
   <si>
-    <t>198.18.193.1</t>
-  </si>
-  <si>
     <t>VLAN 102 GW</t>
   </si>
   <si>
-    <t>198.18.193.2</t>
-  </si>
-  <si>
-    <t>198.18.193.3</t>
-  </si>
-  <si>
-    <t>198.18.193.4</t>
-  </si>
-  <si>
-    <t>198.18.193.5</t>
-  </si>
-  <si>
-    <t>198.18.193.6</t>
-  </si>
-  <si>
-    <t>198.18.193.7</t>
-  </si>
-  <si>
-    <t>198.18.193.8</t>
-  </si>
-  <si>
-    <t>198.18.193.9</t>
-  </si>
-  <si>
-    <t>198.18.193.10</t>
-  </si>
-  <si>
-    <t>198.18.193.11</t>
-  </si>
-  <si>
-    <t>198.18.193.12</t>
-  </si>
-  <si>
-    <t>198.18.193.13</t>
-  </si>
-  <si>
-    <t>198.18.193.14</t>
-  </si>
-  <si>
-    <t>198.18.193.15</t>
-  </si>
-  <si>
-    <t>198.18.193.16</t>
-  </si>
-  <si>
-    <t>198.18.193.17</t>
-  </si>
-  <si>
-    <t>198.18.193.18</t>
-  </si>
-  <si>
-    <t>198.18.193.19</t>
-  </si>
-  <si>
-    <t>198.18.193.20</t>
-  </si>
-  <si>
-    <t>198.18.193.21</t>
-  </si>
-  <si>
     <t>DC2-VBGW-1</t>
   </si>
   <si>
@@ -240,6 +108,93 @@
   </si>
   <si>
     <t>CREDENTIALS</t>
+  </si>
+  <si>
+    <t>198.18.101.1</t>
+  </si>
+  <si>
+    <t>198.18.101.2</t>
+  </si>
+  <si>
+    <t>198.18.101.3</t>
+  </si>
+  <si>
+    <t>198.18.101.4</t>
+  </si>
+  <si>
+    <t>198.18.101.5</t>
+  </si>
+  <si>
+    <t>198.18.101.6</t>
+  </si>
+  <si>
+    <t>198.18.101.7</t>
+  </si>
+  <si>
+    <t>198.18.101.8</t>
+  </si>
+  <si>
+    <t>198.18.101.9</t>
+  </si>
+  <si>
+    <t>198.18.101.10</t>
+  </si>
+  <si>
+    <t>198.18.101.11</t>
+  </si>
+  <si>
+    <t>198.18.101.12</t>
+  </si>
+  <si>
+    <t>198.18.101.13</t>
+  </si>
+  <si>
+    <t>198.18.101.14</t>
+  </si>
+  <si>
+    <t>198.18.101.15</t>
+  </si>
+  <si>
+    <t>198.18.102.1</t>
+  </si>
+  <si>
+    <t>198.18.102.2</t>
+  </si>
+  <si>
+    <t>198.18.102.3</t>
+  </si>
+  <si>
+    <t>198.18.102.4</t>
+  </si>
+  <si>
+    <t>198.18.102.5</t>
+  </si>
+  <si>
+    <t>198.18.102.6</t>
+  </si>
+  <si>
+    <t>198.18.102.7</t>
+  </si>
+  <si>
+    <t>198.18.102.8</t>
+  </si>
+  <si>
+    <t>198.18.102.9</t>
+  </si>
+  <si>
+    <t>198.18.102.10</t>
+  </si>
+  <si>
+    <t>198.18.102.11</t>
+  </si>
+  <si>
+    <t>198.18.102.12</t>
+  </si>
+  <si>
+    <t>198.18.102.13</t>
+  </si>
+  <si>
+    <t>198.18.101.254</t>
   </si>
 </sst>
 </file>
@@ -618,328 +573,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7CAAB7-B9E7-5749-A121-5CC9BF122BDA}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F22" sqref="A1:F22"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>57</v>
+      <c r="C18" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>